<commit_message>
Started ignoring some columns that can be computed/inferred from other columns in the order and truck sheets
These columns are order_number, service_time, latest_dep_time and truck_s_number.

NOTE: If your database (SQLite) is on the latest version before this commit, run `flask db downgrade` and `flask db upgrade`
</commit_message>
<xml_diff>
--- a/tests/data/truck_availability_duplicate_columns.xlsx
+++ b/tests/data/truck_availability_duplicate_columns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bestanden\1-SEP TRUCK\sep-2021_q1-group-2\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Python code\SEP\sep-2021_q1-group-2\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCCDC69D-226A-4C27-8FFE-7FE400AC1D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F958360-7DCD-408C-88C0-821D112136E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23805" yWindow="4620" windowWidth="9870" windowHeight="8055" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="130">
   <si>
     <t>Truck ID</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Driver_thi</t>
   </si>
   <si>
-    <t>V15</t>
-  </si>
-  <si>
     <t>Driver_Pie</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
   </si>
   <si>
     <t>Driver_Blaise</t>
-  </si>
-  <si>
-    <t>V25</t>
   </si>
   <si>
     <t>Driver_man</t>
@@ -874,7 +868,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +912,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
@@ -1011,7 +1005,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
@@ -1242,7 +1236,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4">
         <v>6</v>
@@ -1257,7 +1251,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>15</v>
@@ -1280,7 +1274,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
@@ -1295,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>15</v>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
@@ -1333,7 +1327,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>15</v>
@@ -1356,7 +1350,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
@@ -1371,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>15</v>
@@ -1394,7 +1388,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
@@ -1409,7 +1403,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>15</v>
@@ -1432,7 +1426,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
@@ -1441,13 +1435,13 @@
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>15</v>
@@ -1470,22 +1464,22 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="4">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="4">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>15</v>
@@ -1508,7 +1502,7 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4">
         <v>16</v>
@@ -1517,13 +1511,13 @@
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>15</v>
@@ -1546,7 +1540,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4">
         <v>17</v>
@@ -1555,13 +1549,13 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>15</v>
@@ -1584,7 +1578,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="4">
         <v>18</v>
@@ -1599,7 +1593,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>15</v>
@@ -1622,7 +1616,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1637,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>15</v>
@@ -1660,7 +1654,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
@@ -1669,13 +1663,13 @@
         <v>13</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>15</v>
@@ -1698,7 +1692,7 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="4">
         <v>21</v>
@@ -1707,13 +1701,13 @@
         <v>13</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>15</v>
@@ -1736,7 +1730,7 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="4">
         <v>22</v>
@@ -1751,7 +1745,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>15</v>
@@ -1774,7 +1768,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="4">
         <v>23</v>
@@ -1789,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>15</v>
@@ -1812,7 +1806,7 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
@@ -1827,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>15</v>
@@ -1850,7 +1844,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" s="4">
         <v>25</v>
@@ -1865,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>15</v>
@@ -1888,7 +1882,7 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B27" s="4">
         <v>26</v>
@@ -1897,13 +1891,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>15</v>
@@ -1926,7 +1920,7 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="4">
         <v>26</v>
@@ -1935,13 +1929,13 @@
         <v>13</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>15</v>
@@ -1964,7 +1958,7 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="4">
         <v>28</v>
@@ -1973,13 +1967,13 @@
         <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>15</v>
@@ -2002,7 +1996,7 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" s="4">
         <v>29</v>
@@ -2011,13 +2005,13 @@
         <v>13</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>15</v>
@@ -2040,7 +2034,7 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="4">
         <v>30</v>
@@ -2055,7 +2049,7 @@
         <v>15</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>15</v>
@@ -2078,7 +2072,7 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="4">
         <v>31</v>
@@ -2093,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>15</v>
@@ -2116,7 +2110,7 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" s="4">
         <v>32</v>
@@ -2128,16 +2122,16 @@
         <v>24</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="I33" s="5">
         <v>2</v>
@@ -2154,7 +2148,7 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B34" s="4">
         <v>33</v>
@@ -2166,16 +2160,16 @@
         <v>24</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="I34" s="5">
         <v>2</v>
@@ -2192,7 +2186,7 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" s="4">
         <v>34</v>
@@ -2204,16 +2198,16 @@
         <v>24</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I35" s="5">
         <v>2</v>
@@ -2230,7 +2224,7 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -2239,19 +2233,19 @@
         <v>13</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I36" s="5">
         <v>3</v>
@@ -2268,7 +2262,7 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B37" s="4">
         <v>36</v>
@@ -2280,16 +2274,16 @@
         <v>24</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I37" s="5">
         <v>3</v>
@@ -2306,7 +2300,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4">
         <v>37</v>
@@ -2318,16 +2312,16 @@
         <v>24</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I38" s="5">
         <v>3</v>
@@ -2344,28 +2338,28 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="4">
         <v>38</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I39" s="5">
         <v>3</v>
@@ -2382,7 +2376,7 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40" s="4">
         <v>39</v>
@@ -2391,19 +2385,19 @@
         <v>13</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I40" s="5">
         <v>3</v>
@@ -2420,7 +2414,7 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B41" s="4">
         <v>40</v>
@@ -2432,16 +2426,16 @@
         <v>24</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I41" s="5">
         <v>3</v>
@@ -2458,7 +2452,7 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B42" s="4">
         <v>41</v>
@@ -2470,16 +2464,16 @@
         <v>24</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I42" s="5">
         <v>3</v>
@@ -2496,28 +2490,28 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B43" s="4">
         <v>42</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I43" s="5">
         <v>3</v>
@@ -2534,7 +2528,7 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="4">
         <v>43</v>
@@ -2543,19 +2537,19 @@
         <v>13</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I44" s="5">
         <v>3</v>
@@ -2572,7 +2566,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B45" s="4">
         <v>44</v>
@@ -2584,16 +2578,16 @@
         <v>24</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I45" s="5">
         <v>3</v>
@@ -2610,7 +2604,7 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B46" s="4">
         <v>45</v>
@@ -2622,16 +2616,16 @@
         <v>24</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I46" s="5">
         <v>3</v>
@@ -2648,28 +2642,28 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47" s="4">
         <v>46</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I47" s="5">
         <v>3</v>
@@ -2686,28 +2680,28 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B48" s="4">
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I48" s="5">
         <v>3</v>
@@ -2724,28 +2718,28 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4">
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I49" s="5">
         <v>3</v>
@@ -2762,28 +2756,28 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B50" s="4">
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I50" s="5">
         <v>3</v>

</xml_diff>